<commit_message>
Message document update to outline the IANA registry
</commit_message>
<xml_diff>
--- a/TypeNameSpace.xlsx
+++ b/TypeNameSpace.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="22000" yWindow="8740" windowWidth="28800" windowHeight="16400" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="31980" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="83">
   <si>
     <t>Level</t>
   </si>
@@ -66,9 +66,6 @@
     <t>T_OBJHASHRESTR</t>
   </si>
   <si>
-    <t>T_IPIDM</t>
-  </si>
-  <si>
     <t>%x0005</t>
   </si>
   <si>
@@ -156,9 +153,6 @@
     <t>T_VMAC-128</t>
   </si>
   <si>
-    <t>T_RSA=SHA256</t>
-  </si>
-  <si>
     <t>EC-SECP-256K1</t>
   </si>
   <si>
@@ -250,6 +244,30 @@
   </si>
   <si>
     <t>val depdata</t>
+  </si>
+  <si>
+    <t>T_MSGHASH</t>
+  </si>
+  <si>
+    <t>unassigned</t>
+  </si>
+  <si>
+    <t>T_RSA-SHA256</t>
+  </si>
+  <si>
+    <t>HashFunctions</t>
+  </si>
+  <si>
+    <t>T_SHA-256</t>
+  </si>
+  <si>
+    <t>T_SHA-512</t>
+  </si>
+  <si>
+    <t>%x1000 - %x1FFF</t>
+  </si>
+  <si>
+    <t>reserved</t>
   </si>
 </sst>
 </file>
@@ -298,8 +316,134 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -341,7 +485,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="161">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -359,6 +503,69 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -376,6 +583,69 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -705,10 +975,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -717,6 +987,7 @@
     <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="3" width="13.5" customWidth="1"/>
     <col min="4" max="4" width="21.1640625" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" customWidth="1"/>
     <col min="8" max="8" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -731,7 +1002,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -743,12 +1014,12 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -757,24 +1028,24 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -783,24 +1054,24 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -809,24 +1080,24 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" t="s">
         <v>30</v>
-      </c>
-      <c r="G4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -835,38 +1106,38 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="E6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" t="s">
         <v>57</v>
-      </c>
-      <c r="G6" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -875,24 +1146,24 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" t="s">
         <v>35</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>36</v>
-      </c>
-      <c r="H7" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
@@ -901,26 +1172,26 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
@@ -929,390 +1200,432 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F11" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="G11" t="s">
         <v>7</v>
       </c>
       <c r="H11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
         <v>61</v>
       </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" t="s">
-        <v>63</v>
-      </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G12" t="s">
         <v>8</v>
       </c>
       <c r="H12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
         <v>61</v>
       </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" t="s">
-        <v>63</v>
-      </c>
       <c r="F13" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="G13" t="s">
         <v>9</v>
       </c>
       <c r="H13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
         <v>61</v>
       </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" t="s">
-        <v>63</v>
-      </c>
       <c r="F14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G14" t="s">
         <v>10</v>
       </c>
       <c r="H14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" t="s">
         <v>61</v>
       </c>
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" t="s">
-        <v>63</v>
-      </c>
       <c r="F15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" t="s">
         <v>61</v>
       </c>
-      <c r="B16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" t="s">
-        <v>63</v>
-      </c>
       <c r="F16" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="G16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" t="s">
         <v>61</v>
       </c>
-      <c r="B17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" t="s">
-        <v>63</v>
-      </c>
       <c r="F17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" t="s">
         <v>46</v>
       </c>
-      <c r="G17" t="s">
-        <v>48</v>
-      </c>
       <c r="H17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="E18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" t="s">
         <v>47</v>
       </c>
-      <c r="G18" t="s">
-        <v>49</v>
-      </c>
       <c r="H18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
         <v>50</v>
-      </c>
-      <c r="B20" t="s">
-        <v>52</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C22" t="s">
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E22" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F23" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" t="s">
         <v>54</v>
       </c>
-      <c r="C24" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" t="s">
-        <v>56</v>
-      </c>
       <c r="E24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G25" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="E26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G26" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H26" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>